<commit_message>
card stat program finished
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Id</t>
   </si>
@@ -157,6 +157,102 @@
   </si>
   <si>
     <t>--城堡XXXXX</t>
+  </si>
+  <si>
+    <t>嘲讽</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTaunt</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountRush</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountHide</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光环</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountAuro</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountAoe</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AOE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buff</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountBuff</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>克制</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountOver</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>远程</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountRange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountDefend</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountSummon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>过牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountMag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountCard</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -861,12 +957,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:C21" totalsRowShown="0">
-  <autoFilter ref="A3:C21"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:O21" totalsRowShown="0">
+  <autoFilter ref="A3:O21"/>
+  <tableColumns count="15">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Des" dataDxfId="0"/>
+    <tableColumn id="3" name="CountTaunt"/>
+    <tableColumn id="5" name="CountRush"/>
+    <tableColumn id="6" name="CountHide"/>
+    <tableColumn id="7" name="CountAuro"/>
+    <tableColumn id="8" name="CountAoe"/>
+    <tableColumn id="9" name="CountBuff"/>
+    <tableColumn id="10" name="CountOver"/>
+    <tableColumn id="11" name="CountRange"/>
+    <tableColumn id="12" name="CountDefend"/>
+    <tableColumn id="13" name="CountSummon"/>
+    <tableColumn id="14" name="CountMag"/>
+    <tableColumn id="15" name="CountCard"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1193,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C21"/>
+      <selection activeCell="D4" sqref="D4:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1204,9 +1312,12 @@
     <col min="1" max="1" width="5.75" customWidth="1"/>
     <col min="2" max="2" width="9.375" customWidth="1"/>
     <col min="3" max="3" width="31.25" customWidth="1"/>
+    <col min="4" max="7" width="3.875" customWidth="1"/>
+    <col min="8" max="11" width="3.5" customWidth="1"/>
+    <col min="12" max="15" width="3.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1216,8 +1327,44 @@
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1227,8 +1374,44 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1238,8 +1421,44 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1249,8 +1468,44 @@
       <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1260,8 +1515,44 @@
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1271,8 +1562,44 @@
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1282,8 +1609,44 @@
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1293,8 +1656,44 @@
       <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1304,8 +1703,44 @@
       <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1315,8 +1750,44 @@
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1326,8 +1797,44 @@
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1337,8 +1844,44 @@
       <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1348,8 +1891,44 @@
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1359,8 +1938,44 @@
       <c r="C14" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1370,8 +1985,44 @@
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1381,8 +2032,44 @@
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1392,8 +2079,44 @@
       <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1403,8 +2126,44 @@
       <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1414,8 +2173,44 @@
       <c r="C19" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>9</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>34</v>
       </c>
@@ -1426,7 +2221,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>35</v>
       </c>
@@ -1439,9 +2234,124 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="D4:H19">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9DDECB9F-765B-4F73-BD41-1FAB37B60302}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:K19">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E768AECC-328B-4288-9B4C-C3D5C7CC291C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L19">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{90CB5060-4584-4285-AE48-0CE184373E66}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:O19">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{52BD0956-B70C-4EFD-95F8-9DD27D76FCE7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9DDECB9F-765B-4F73-BD41-1FAB37B60302}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D4:H19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E768AECC-328B-4288-9B4C-C3D5C7CC291C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I4:K19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{90CB5060-4584-4285-AE48-0CE184373E66}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L4:L19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{52BD0956-B70C-4EFD-95F8-9DD27D76FCE7}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M4:O19</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
split the DeathSkill form deathhit system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -108,51 +108,15 @@
     <t>--恶魔XXXXX</t>
   </si>
   <si>
-    <t>--机械XXXXX</t>
-  </si>
-  <si>
-    <t>--精灵XXXXX</t>
-  </si>
-  <si>
-    <t>--昆虫XXXXX</t>
-  </si>
-  <si>
-    <t>--龙XXXXX</t>
-  </si>
-  <si>
-    <t>--鸟XXXXX</t>
-  </si>
-  <si>
     <t>--爬行XXXXX</t>
   </si>
   <si>
-    <t>--人类XXXXX</t>
-  </si>
-  <si>
-    <t>--兽人XXXXX</t>
-  </si>
-  <si>
-    <t>--亡灵XXXXX</t>
-  </si>
-  <si>
     <t>--野兽XXXXX</t>
   </si>
   <si>
     <t>--鱼XXXXX</t>
   </si>
   <si>
-    <t>--元素XXXXX</t>
-  </si>
-  <si>
-    <t>--植物XXXXX</t>
-  </si>
-  <si>
-    <t>--地精XXXXX</t>
-  </si>
-  <si>
-    <t>--石像XXXXX</t>
-  </si>
-  <si>
     <t>--建筑XXXXX</t>
   </si>
   <si>
@@ -252,6 +216,50 @@
   </si>
   <si>
     <t>CountCard</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--身强体壮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长亡语技能$--擅长buff效果</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长防御特质</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长远程攻击$--擅长防御特质</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长范围伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长光环效果</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长快速移动$--擅长冲锋技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长各种高级魔法效果</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长召唤技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长克制技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长远程攻击$--擅长魔法技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -945,6 +953,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -988,7 +1064,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1304,7 +1380,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:O19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1328,40 +1404,40 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -1422,40 +1498,40 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="L3" t="s">
         <v>49</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="N3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" t="s">
         <v>55</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
@@ -1513,7 +1589,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1560,7 +1636,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1607,7 +1683,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1654,7 +1730,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1701,7 +1777,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1748,7 +1824,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1795,7 +1871,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1842,7 +1918,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1889,7 +1965,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1936,7 +2012,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -1983,7 +2059,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2030,7 +2106,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2077,7 +2153,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2124,7 +2200,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2171,7 +2247,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2218,7 +2294,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.15">
@@ -2229,7 +2305,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extend the skill stat
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>Id</t>
   </si>
@@ -260,6 +260,30 @@
   </si>
   <si>
     <t>--擅长远程攻击$--擅长魔法技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡语</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountDeathSay</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>支援</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountHeal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountAid</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1033,9 +1057,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:O21" totalsRowShown="0">
-  <autoFilter ref="A3:O21"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:R21" totalsRowShown="0">
+  <autoFilter ref="A3:R21"/>
+  <tableColumns count="18">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Des" dataDxfId="0"/>
@@ -1051,6 +1075,9 @@
     <tableColumn id="13" name="CountSummon"/>
     <tableColumn id="14" name="CountMag"/>
     <tableColumn id="15" name="CountCard"/>
+    <tableColumn id="16" name="CountDeathSay"/>
+    <tableColumn id="17" name="CountHeal"/>
+    <tableColumn id="18" name="CountAid"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1377,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D4" sqref="D4:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1388,12 +1415,10 @@
     <col min="1" max="1" width="5.75" customWidth="1"/>
     <col min="2" max="2" width="9.375" customWidth="1"/>
     <col min="3" max="3" width="31.25" customWidth="1"/>
-    <col min="4" max="7" width="3.875" customWidth="1"/>
-    <col min="8" max="11" width="3.5" customWidth="1"/>
-    <col min="12" max="15" width="3.25" customWidth="1"/>
+    <col min="4" max="18" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1439,8 +1464,17 @@
       <c r="O1" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1486,8 +1520,17 @@
       <c r="O2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="P2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1533,8 +1576,17 @@
       <c r="O3" t="s">
         <v>55</v>
       </c>
+      <c r="P3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1578,10 +1630,19 @@
         <v>4</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1627,8 +1688,17 @@
       <c r="O5">
         <v>0</v>
       </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1648,10 +1718,10 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1674,8 +1744,17 @@
       <c r="O6">
         <v>0</v>
       </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1713,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1721,8 +1800,17 @@
       <c r="O7">
         <v>0</v>
       </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1742,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -1768,8 +1856,17 @@
       <c r="O8">
         <v>1</v>
       </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1815,8 +1912,17 @@
       <c r="O9">
         <v>0</v>
       </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1839,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -1862,8 +1968,17 @@
       <c r="O10">
         <v>0</v>
       </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1886,7 +2001,7 @@
         <v>3</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -1901,16 +2016,25 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1954,10 +2078,19 @@
         <v>3</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1980,10 +2113,10 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -2001,10 +2134,19 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2024,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2050,8 +2192,17 @@
       <c r="O14">
         <v>0</v>
       </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2092,13 +2243,22 @@
         <v>1</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2144,8 +2304,17 @@
       <c r="O16">
         <v>0</v>
       </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2168,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -2191,8 +2360,17 @@
       <c r="O17">
         <v>0</v>
       </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>3</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2212,7 +2390,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>3</v>
@@ -2238,8 +2416,17 @@
       <c r="O18">
         <v>3</v>
       </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2259,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2283,10 +2470,19 @@
         <v>0</v>
       </c>
       <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>34</v>
       </c>
@@ -2297,7 +2493,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>35</v>
       </c>
@@ -2311,7 +2507,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:H19">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2325,7 +2521,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:K19">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2339,7 +2535,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L19">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2353,6 +2549,48 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:O19">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{52BD0956-B70C-4EFD-95F8-9DD27D76FCE7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P19">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8C174AC0-88D0-4595-8353-C2E952BC4D0F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:Q19">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3141DB82-1812-442A-9489-0E2144253DC2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R19">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -2361,7 +2599,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52BD0956-B70C-4EFD-95F8-9DD27D76FCE7}</x14:id>
+          <x14:id>{6FA1EFF6-9E31-4649-B2BE-92B57AEAF144}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2426,6 +2664,45 @@
           </x14:cfRule>
           <xm:sqref>M4:O19</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8C174AC0-88D0-4595-8353-C2E952BC4D0F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P4:P19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3141DB82-1812-442A-9489-0E2144253DC2}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>Q4:Q19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6FA1EFF6-9E31-4649-B2BE-92B57AEAF144}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R4:R19</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
optimise card attr showing
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>Id</t>
   </si>
@@ -284,6 +284,10 @@
   </si>
   <si>
     <t>CountAid</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长远程攻击$--擅长各种技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1986,7 +1990,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2284,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -2506,7 +2510,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:H19">
+  <conditionalFormatting sqref="D4:R19">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
@@ -2516,90 +2520,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{9DDECB9F-765B-4F73-BD41-1FAB37B60302}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:K19">
-    <cfRule type="dataBar" priority="6">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E768AECC-328B-4288-9B4C-C3D5C7CC291C}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L19">
-    <cfRule type="dataBar" priority="5">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{90CB5060-4584-4285-AE48-0CE184373E66}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M4:O19">
-    <cfRule type="dataBar" priority="4">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52BD0956-B70C-4EFD-95F8-9DD27D76FCE7}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P19">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8C174AC0-88D0-4595-8353-C2E952BC4D0F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q4:Q19">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3141DB82-1812-442A-9489-0E2144253DC2}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4:R19">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6FA1EFF6-9E31-4649-B2BE-92B57AEAF144}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2623,85 +2543,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D4:H19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E768AECC-328B-4288-9B4C-C3D5C7CC291C}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>I4:K19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{90CB5060-4584-4285-AE48-0CE184373E66}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>L4:L19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{52BD0956-B70C-4EFD-95F8-9DD27D76FCE7}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M4:O19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8C174AC0-88D0-4595-8353-C2E952BC4D0F}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>P4:P19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3141DB82-1812-442A-9489-0E2144253DC2}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>Q4:Q19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6FA1EFF6-9E31-4649-B2BE-92B57AEAF144}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>R4:R19</xm:sqref>
+          <xm:sqref>D4:R19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
optimise the buff immune system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -243,10 +243,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长快速移动$--擅长冲锋技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>--擅长各种高级魔法效果</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -288,6 +284,10 @@
   </si>
   <si>
     <t>--擅长远程攻击$--擅长各种技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长克制技能$--擅长冲锋技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1469,13 +1469,13 @@
         <v>53</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -1581,13 +1581,13 @@
         <v>55</v>
       </c>
       <c r="P3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" t="s">
         <v>71</v>
-      </c>
-      <c r="R3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -1654,7 +1654,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1710,7 +1710,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1725,7 +1725,7 @@
         <v>2</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1766,7 +1766,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1822,7 +1822,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1878,13 +1878,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1899,7 +1899,7 @@
         <v>2</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1920,7 +1920,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1990,7 +1990,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2341,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <v>3</v>

</xml_diff>

<commit_message>
set the race resist attr
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>Id</t>
   </si>
@@ -239,10 +239,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长光环效果</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>--擅长各种高级魔法效果</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -288,6 +284,18 @@
   </si>
   <si>
     <t>--擅长克制技能$--擅长冲锋技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>规则</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountRule</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长规则技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1061,9 +1069,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:R21" totalsRowShown="0">
-  <autoFilter ref="A3:R21"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S21" totalsRowShown="0">
+  <autoFilter ref="A3:S21"/>
+  <tableColumns count="19">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Des" dataDxfId="0"/>
@@ -1082,6 +1090,7 @@
     <tableColumn id="16" name="CountDeathSay"/>
     <tableColumn id="17" name="CountHeal"/>
     <tableColumn id="18" name="CountAid"/>
+    <tableColumn id="19" name="CountRule"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1408,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:R19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1419,10 +1428,11 @@
     <col min="1" max="1" width="5.75" customWidth="1"/>
     <col min="2" max="2" width="9.375" customWidth="1"/>
     <col min="3" max="3" width="31.25" customWidth="1"/>
-    <col min="4" max="18" width="4" customWidth="1"/>
+    <col min="4" max="17" width="4" customWidth="1"/>
+    <col min="18" max="19" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1469,16 +1479,19 @@
         <v>53</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>69</v>
+      <c r="S1" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1533,8 +1546,11 @@
       <c r="R2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="S2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1581,16 +1597,19 @@
         <v>55</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" t="s">
         <v>70</v>
       </c>
-      <c r="R3" t="s">
-        <v>71</v>
+      <c r="S3" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1645,8 +1664,11 @@
       <c r="R4">
         <v>6</v>
       </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1654,7 +1676,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1701,8 +1723,11 @@
       <c r="R5">
         <v>0</v>
       </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1710,7 +1735,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1757,8 +1782,11 @@
       <c r="R6">
         <v>1</v>
       </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1766,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1813,8 +1841,11 @@
       <c r="R7">
         <v>1</v>
       </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1822,7 +1853,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1869,8 +1900,11 @@
       <c r="R8">
         <v>0</v>
       </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1878,7 +1912,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1925,8 +1959,11 @@
       <c r="R9">
         <v>0</v>
       </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1981,8 +2018,11 @@
       <c r="R10">
         <v>0</v>
       </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1990,7 +2030,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2037,8 +2077,11 @@
       <c r="R11">
         <v>4</v>
       </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2093,8 +2136,11 @@
       <c r="R12">
         <v>1</v>
       </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2149,8 +2195,11 @@
       <c r="R13">
         <v>3</v>
       </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2205,8 +2254,11 @@
       <c r="R14">
         <v>1</v>
       </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2261,8 +2313,11 @@
       <c r="R15">
         <v>1</v>
       </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2317,8 +2372,11 @@
       <c r="R16">
         <v>0</v>
       </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2373,8 +2431,11 @@
       <c r="R17">
         <v>1</v>
       </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2429,8 +2490,11 @@
       <c r="R18">
         <v>0</v>
       </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2438,7 +2502,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2485,8 +2549,11 @@
       <c r="R19">
         <v>0</v>
       </c>
+      <c r="S19">
+        <v>7</v>
+      </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>34</v>
       </c>
@@ -2497,7 +2564,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>35</v>
       </c>
@@ -2511,7 +2578,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:R19">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2520,6 +2587,20 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{9DDECB9F-765B-4F73-BD41-1FAB37B60302}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4:S19">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{75966C34-D02D-4A6A-AC2B-18D86504559B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2545,6 +2626,19 @@
           </x14:cfRule>
           <xm:sqref>D4:R19</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{75966C34-D02D-4A6A-AC2B-18D86504559B}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S4:S19</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
optimise the machine cards skills
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -247,10 +247,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长克制技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>--擅长远程攻击$--擅长魔法技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -296,6 +292,10 @@
   </si>
   <si>
     <t>--擅长规则技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长攻城$--擅长抵抗远程</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -989,74 +989,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1104,7 +1036,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1420,7 +1352,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1479,16 +1411,16 @@
         <v>53</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="S1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -1597,16 +1529,16 @@
         <v>55</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" t="s">
         <v>69</v>
       </c>
-      <c r="R3" t="s">
-        <v>70</v>
-      </c>
       <c r="S3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -1676,7 +1608,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1735,7 +1667,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1912,7 +1844,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2030,7 +1962,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2502,7 +2434,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19">
         <v>0</v>

</xml_diff>

<commit_message>
fix the attr skill of birds
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
   <si>
     <t>Id</t>
   </si>
@@ -296,6 +296,14 @@
   </si>
   <si>
     <t>--擅长攻城$--擅长抵抗远程</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻城</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTank</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -483,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,6 +674,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,7 +939,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -936,6 +950,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1001,9 +1018,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S21" totalsRowShown="0">
-  <autoFilter ref="A3:S21"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T21" totalsRowShown="0">
+  <autoFilter ref="A3:T21"/>
+  <tableColumns count="20">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Des" dataDxfId="0"/>
@@ -1023,6 +1040,7 @@
     <tableColumn id="17" name="CountHeal"/>
     <tableColumn id="18" name="CountAid"/>
     <tableColumn id="19" name="CountRule"/>
+    <tableColumn id="20" name="CountTank"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1349,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1360,11 +1378,10 @@
     <col min="1" max="1" width="5.75" customWidth="1"/>
     <col min="2" max="2" width="9.375" customWidth="1"/>
     <col min="3" max="3" width="31.25" customWidth="1"/>
-    <col min="4" max="17" width="4" customWidth="1"/>
-    <col min="18" max="19" width="3.625" customWidth="1"/>
+    <col min="4" max="20" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1422,8 +1439,11 @@
       <c r="S1" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1481,8 +1501,11 @@
       <c r="S2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1540,8 +1563,11 @@
       <c r="S3" t="s">
         <v>73</v>
       </c>
+      <c r="T3" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1599,19 +1625,22 @@
       <c r="S4">
         <v>1</v>
       </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1632,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -1658,8 +1687,11 @@
       <c r="S5">
         <v>1</v>
       </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1717,8 +1749,11 @@
       <c r="S6">
         <v>1</v>
       </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1776,8 +1811,11 @@
       <c r="S7">
         <v>0</v>
       </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1835,22 +1873,25 @@
       <c r="S8">
         <v>2</v>
       </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1894,8 +1935,11 @@
       <c r="S9">
         <v>0</v>
       </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1953,8 +1997,11 @@
       <c r="S10">
         <v>0</v>
       </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2012,8 +2059,11 @@
       <c r="S11">
         <v>0</v>
       </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2071,8 +2121,11 @@
       <c r="S12">
         <v>0</v>
       </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2130,8 +2183,11 @@
       <c r="S13">
         <v>0</v>
       </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2189,8 +2245,11 @@
       <c r="S14">
         <v>1</v>
       </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2248,8 +2307,11 @@
       <c r="S15">
         <v>0</v>
       </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2307,8 +2369,11 @@
       <c r="S16">
         <v>2</v>
       </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2366,8 +2431,11 @@
       <c r="S17">
         <v>0</v>
       </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2425,8 +2493,11 @@
       <c r="S18">
         <v>1</v>
       </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2484,8 +2555,11 @@
       <c r="S19">
         <v>7</v>
       </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>34</v>
       </c>
@@ -2496,7 +2570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>35</v>
       </c>
@@ -2523,7 +2597,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S19">
+  <conditionalFormatting sqref="S4:T19">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -2569,7 +2643,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>S4:S19</xm:sqref>
+          <xm:sqref>S4:T19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
new element combo mark effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -312,7 +312,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长怒火技能</t>
+    <t>--擅长怒火技能$--体格强壮</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1015,6 +1015,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1064,7 +1132,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2113,7 +2181,7 @@
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D12">

</xml_diff>

<commit_message>
finish the element skill config
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -213,10 +213,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长防御特质</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>--擅长远程攻击$--擅长防御特质</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -321,6 +317,18 @@
   </si>
   <si>
     <t>CountElement</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地形</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTile</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长防御特质$--擅长元素技能</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1035,9 +1043,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:V21" totalsRowShown="0">
-  <autoFilter ref="A3:V21"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:W21" totalsRowShown="0">
+  <autoFilter ref="A3:W21"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Des" dataDxfId="0"/>
@@ -1060,6 +1068,7 @@
     <tableColumn id="20" name="CountTank"/>
     <tableColumn id="21" name="CountTank2"/>
     <tableColumn id="22" name="CountElement"/>
+    <tableColumn id="23" name="CountTile"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1386,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1398,10 +1407,11 @@
     <col min="2" max="2" width="9.375" customWidth="1"/>
     <col min="3" max="3" width="31.25" customWidth="1"/>
     <col min="4" max="20" width="3.75" customWidth="1"/>
-    <col min="21" max="22" width="3.875" customWidth="1"/>
+    <col min="21" max="21" width="3.875" customWidth="1"/>
+    <col min="22" max="23" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1448,28 +1458,31 @@
         <v>51</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="S1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1536,8 +1549,11 @@
       <c r="V2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="W2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1584,28 +1600,31 @@
         <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
         <v>62</v>
       </c>
-      <c r="R3" t="s">
-        <v>63</v>
-      </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V3" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="W3" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1613,7 +1632,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1672,8 +1691,11 @@
       <c r="V4">
         <v>0</v>
       </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1681,7 +1703,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1735,13 +1757,16 @@
         <v>4</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <v>0</v>
       </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1749,7 +1774,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1808,8 +1833,11 @@
       <c r="V6">
         <v>0</v>
       </c>
+      <c r="W6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1817,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1876,8 +1904,11 @@
       <c r="V7">
         <v>0</v>
       </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1885,7 +1916,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1939,13 +1970,16 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1953,7 +1987,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2012,8 +2046,11 @@
       <c r="V9">
         <v>0</v>
       </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2021,7 +2058,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2075,13 +2112,16 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2089,7 +2129,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2146,10 +2186,13 @@
         <v>4</v>
       </c>
       <c r="V11">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2157,7 +2200,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2214,10 +2257,13 @@
         <v>5</v>
       </c>
       <c r="V12">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2225,7 +2271,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2284,8 +2330,11 @@
       <c r="V13">
         <v>0</v>
       </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2347,13 +2396,16 @@
         <v>0</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <v>0</v>
       </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2420,16 +2472,19 @@
       <c r="V15">
         <v>0</v>
       </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>54</v>
+      <c r="C16" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -2486,10 +2541,13 @@
         <v>0</v>
       </c>
       <c r="V16">
+        <v>7</v>
+      </c>
+      <c r="W16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2497,7 +2555,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2556,8 +2614,11 @@
       <c r="V17">
         <v>0</v>
       </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2565,7 +2626,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2624,8 +2685,11 @@
       <c r="V18">
         <v>0</v>
       </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2633,7 +2697,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2692,8 +2756,11 @@
       <c r="V19">
         <v>0</v>
       </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>34</v>
       </c>
@@ -2704,7 +2771,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>35</v>
       </c>
@@ -2717,8 +2784,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:U19">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="D4:W19">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2727,20 +2794,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{9DDECB9F-765B-4F73-BD41-1FAB37B60302}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V4:V19">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7DE0F79F-8CDF-4DF8-8C2C-6A423779D717}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2764,20 +2817,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D4:U19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7DE0F79F-8CDF-4DF8-8C2C-6A423779D717}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>V4:V19</xm:sqref>
+          <xm:sqref>D4:W19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
finish the undie cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -1398,7 +1398,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2270,7 +2270,7 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D13">
@@ -2283,13 +2283,13 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -2301,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="M13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2310,7 +2310,7 @@
         <v>3</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q13">
         <v>1</v>

</xml_diff>

<commit_message>
finish the fish cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -108,9 +108,6 @@
     <t>--野兽XXXXX</t>
   </si>
   <si>
-    <t>--鱼XXXXX</t>
-  </si>
-  <si>
     <t>--建筑XXXXX</t>
   </si>
   <si>
@@ -329,6 +326,10 @@
   </si>
   <si>
     <t>--擅长防御特质$--擅长元素技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>--擅长支援</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1398,7 +1399,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D4" sqref="D4:W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1422,64 +1423,64 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="S1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
@@ -1564,64 +1565,64 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
       <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" t="s">
         <v>52</v>
       </c>
-      <c r="O3" t="s">
-        <v>53</v>
-      </c>
       <c r="P3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" t="s">
         <v>61</v>
       </c>
-      <c r="R3" t="s">
-        <v>62</v>
-      </c>
       <c r="S3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.15">
@@ -1632,7 +1633,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1703,7 +1704,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1774,7 +1775,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1845,7 +1846,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1916,7 +1917,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1987,7 +1988,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2058,7 +2059,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2129,7 +2130,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2200,7 +2201,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2271,7 +2272,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2412,8 +2413,8 @@
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
+      <c r="C15" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2458,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -2484,7 +2485,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -2555,7 +2556,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2626,7 +2627,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2697,7 +2698,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2768,7 +2769,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.15">
@@ -2779,7 +2780,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish race card balance
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MonsterRace.xlsx
+++ b/ConfigData/Xlsx/MonsterRace.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>Id</t>
   </si>
@@ -105,15 +105,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--野兽XXXXX</t>
-  </si>
-  <si>
-    <t>--建筑XXXXX</t>
-  </si>
-  <si>
-    <t>--城堡XXXXX</t>
-  </si>
-  <si>
     <t>嘲讽</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -210,18 +201,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长远程攻击$--擅长防御特质</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长范围伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长各种高级魔法效果</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>亡语</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -246,14 +225,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长远程攻击$--擅长各种技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长克制技能$--擅长冲锋技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>规则</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -262,14 +233,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长规则技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长攻城$--擅长抵抗远程</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>攻城</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -278,26 +241,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长召唤技能$--高闪避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长buff技能$--高暴击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长亡语技能$--擅长buff技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长远程攻击$--擅长魔法</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长buff技能$--高物理输出</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>CountTank2</t>
   </si>
   <si>
@@ -305,10 +248,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长怒火技能$--体格强壮</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>元素</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -325,12 +264,64 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>--擅长防御特质$--擅长元素技能</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>--擅长支援</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>必杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountKill</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>擅长buff技能$高暴击</t>
+  </si>
+  <si>
+    <t>擅长攻城$擅长抵抗远程</t>
+  </si>
+  <si>
+    <t>擅长远程攻击$擅长魔法</t>
+  </si>
+  <si>
+    <t>擅长召唤技能$高闪避</t>
+  </si>
+  <si>
+    <t>擅长伤害魔法$总属性强大</t>
+  </si>
+  <si>
+    <t>擅长克制技能$擅长冲锋技能</t>
+  </si>
+  <si>
+    <t>擅长buff技能$高物理输出</t>
+  </si>
+  <si>
+    <t>擅长远程攻击$擅长辅助魔法</t>
+  </si>
+  <si>
+    <t>擅长怒火技能$体格强壮</t>
+  </si>
+  <si>
+    <t>擅长亡语技能$擅长buff技能</t>
+  </si>
+  <si>
+    <t>掌握各种技能</t>
+  </si>
+  <si>
+    <t>擅长支援</t>
+  </si>
+  <si>
+    <t>擅长防御特质$擅长元素技能</t>
+  </si>
+  <si>
+    <t>擅长回复技能$擅长防御特质</t>
+  </si>
+  <si>
+    <t>擅长各种发明</t>
+  </si>
+  <si>
+    <t>擅长规则技能</t>
   </si>
 </sst>
 </file>
@@ -517,7 +508,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,14 +694,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -836,6 +821,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -965,7 +959,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -978,7 +972,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1044,9 +1041,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:W21" totalsRowShown="0">
-  <autoFilter ref="A3:W21"/>
-  <tableColumns count="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X21" totalsRowShown="0">
+  <autoFilter ref="A3:X21"/>
+  <tableColumns count="24">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Des" dataDxfId="0"/>
@@ -1070,6 +1067,7 @@
     <tableColumn id="21" name="CountTank2"/>
     <tableColumn id="22" name="CountElement"/>
     <tableColumn id="23" name="CountTile"/>
+    <tableColumn id="24" name="CountKill"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1396,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:W19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1409,10 +1407,11 @@
     <col min="3" max="3" width="31.25" customWidth="1"/>
     <col min="4" max="20" width="3.75" customWidth="1"/>
     <col min="21" max="21" width="3.875" customWidth="1"/>
-    <col min="22" max="23" width="3.75" customWidth="1"/>
+    <col min="22" max="22" width="3.75" customWidth="1"/>
+    <col min="23" max="24" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1423,67 +1422,70 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>80</v>
+      <c r="X1" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1553,8 +1555,11 @@
       <c r="W2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="X2" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1565,75 +1570,78 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" t="s">
         <v>48</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" t="s">
         <v>51</v>
       </c>
-      <c r="O3" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" t="s">
         <v>60</v>
       </c>
-      <c r="R3" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" t="s">
         <v>65</v>
       </c>
-      <c r="T3" t="s">
-        <v>69</v>
-      </c>
-      <c r="U3" t="s">
-        <v>75</v>
-      </c>
-      <c r="V3" t="s">
-        <v>79</v>
-      </c>
-      <c r="W3" t="s">
-        <v>81</v>
+      <c r="X3" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>71</v>
+      <c r="C4" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1695,16 +1703,19 @@
       <c r="W4">
         <v>0</v>
       </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>67</v>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1766,16 +1777,19 @@
       <c r="W5">
         <v>0</v>
       </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>73</v>
+      <c r="C6" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1837,16 +1851,19 @@
       <c r="W6">
         <v>3</v>
       </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>70</v>
+      <c r="C7" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1908,8 +1925,11 @@
       <c r="W7">
         <v>0</v>
       </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1917,7 +1937,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1979,16 +1999,19 @@
       <c r="W8">
         <v>0</v>
       </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>63</v>
+      <c r="C9" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2050,16 +2073,19 @@
       <c r="W9">
         <v>1</v>
       </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>74</v>
+      <c r="C10" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2121,8 +2147,11 @@
       <c r="W10">
         <v>1</v>
       </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2130,7 +2159,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2192,15 +2221,18 @@
       <c r="W11">
         <v>0</v>
       </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D12">
@@ -2263,16 +2295,19 @@
       <c r="W12">
         <v>0</v>
       </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>72</v>
+      <c r="C13" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2334,8 +2369,11 @@
       <c r="W13">
         <v>1</v>
       </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2343,7 +2381,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2405,16 +2443,19 @@
       <c r="W14">
         <v>1</v>
       </c>
+      <c r="X14">
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>83</v>
+      <c r="C15" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2476,16 +2517,19 @@
       <c r="W15">
         <v>1</v>
       </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>82</v>
+      <c r="C16" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -2547,8 +2591,11 @@
       <c r="W16">
         <v>0</v>
       </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2556,7 +2603,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2618,8 +2665,11 @@
       <c r="W17">
         <v>0</v>
       </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2627,7 +2677,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2689,8 +2739,11 @@
       <c r="W18">
         <v>0</v>
       </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2698,7 +2751,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2760,32 +2813,31 @@
       <c r="W19">
         <v>0</v>
       </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="C21" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:W19">
+  <conditionalFormatting sqref="D4:X19">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
@@ -2818,7 +2870,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D4:W19</xm:sqref>
+          <xm:sqref>D4:X19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>